<commit_message>
Bug fix in the PS table v1_0_1
</commit_message>
<xml_diff>
--- a/development/L1Menu_Collisions2022_v1_0_1/PrescaleTable/L1Menu_Collisions2022_v1_0_1.xlsx
+++ b/development/L1Menu_Collisions2022_v1_0_1/PrescaleTable/L1Menu_Collisions2022_v1_0_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caterinaaruta/Desktop/L1Menus/L1Menu_Collisions2022_v1_0_1/PrescaleTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4A71268-C6CF-A94C-B6A9-EBE369DD3F6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05B70C7E-9824-DA46-A827-9B593469C0A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="-17200" windowWidth="29500" windowHeight="16780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-900" yWindow="-19340" windowWidth="30080" windowHeight="19020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -2583,8 +2583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF3B8E07-BE26-384A-A4B5-1B0A96E53592}">
   <dimension ref="A1:IV388"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -14671,7 +14671,7 @@
     </row>
     <row r="346" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A346" s="5">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="B346" s="6" t="s">
         <v>311</v>
@@ -14706,7 +14706,7 @@
     </row>
     <row r="347" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A347" s="5">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="B347" s="6" t="s">
         <v>312</v>
@@ -14741,7 +14741,7 @@
     </row>
     <row r="348" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A348" s="5">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="B348" s="6" t="s">
         <v>313</v>
@@ -14776,7 +14776,7 @@
     </row>
     <row r="349" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A349" s="5">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="B349" s="6" t="s">
         <v>314</v>

</xml_diff>